<commit_message>
identical markdown report generation
</commit_message>
<xml_diff>
--- a/feedback_report.xlsx
+++ b/feedback_report.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7877" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7877" uniqueCount="100">
   <si>
     <t>Year</t>
   </si>
@@ -304,22 +304,25 @@
     <t>Faculty_Initial</t>
   </si>
   <si>
-    <t>JC</t>
+    <t>NJC</t>
   </si>
   <si>
-    <t>KP</t>
+    <t>LKP</t>
   </si>
   <si>
-    <t>PJ</t>
+    <t>SPJ</t>
   </si>
   <si>
-    <t>CP</t>
+    <t>RCP</t>
   </si>
   <si>
-    <t>JD</t>
+    <t>MKP</t>
   </si>
   <si>
-    <t>NP</t>
+    <t>MJD</t>
+  </si>
+  <si>
+    <t>RNP</t>
   </si>
 </sst>
 </file>
@@ -26056,7 +26059,7 @@
         <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C6">
         <v>4.653899240855763</v>
@@ -26103,7 +26106,7 @@
         <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C7">
         <v>4.77938808373591</v>
@@ -26150,7 +26153,7 @@
         <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C8">
         <v>4.750679347826087</v>

</xml_diff>